<commit_message>
Bytt ut Jakriborg mot Värpinge By, närmare centrum
</commit_message>
<xml_diff>
--- a/sql-scripts/station.xlsx
+++ b/sql-scripts/station.xlsx
@@ -83,9 +83,6 @@
     <t>Victoriastadion</t>
   </si>
   <si>
-    <t>Jakriborg</t>
-  </si>
-  <si>
     <t>Kungsmarken</t>
   </si>
   <si>
@@ -138,6 +135,9 @@
   </si>
   <si>
     <t>Bergsbrunnaparken</t>
+  </si>
+  <si>
+    <t>Värpinge By</t>
   </si>
 </sst>
 </file>
@@ -458,7 +458,7 @@
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -750,13 +750,13 @@
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="D13">
-        <v>55.690916399999999</v>
+        <v>55.7010352</v>
       </c>
       <c r="E13">
-        <v>13.1331062</v>
+        <v>13.166274100000001</v>
       </c>
       <c r="F13">
         <v>2E-3</v>
@@ -773,7 +773,7 @@
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D14">
         <v>55.710456600000001</v>
@@ -796,7 +796,7 @@
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D15">
         <v>55.687336100000003</v>
@@ -819,7 +819,7 @@
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D16">
         <v>55.712684899999999</v>
@@ -842,7 +842,7 @@
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D17">
         <v>55.703105999999998</v>
@@ -865,7 +865,7 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D18">
         <v>55.720996599999999</v>
@@ -888,7 +888,7 @@
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D19">
         <v>55.695076700000001</v>
@@ -911,7 +911,7 @@
         <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D20">
         <v>55.698172599999999</v>
@@ -934,7 +934,7 @@
         <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D21">
         <v>55.721532400000001</v>
@@ -957,7 +957,7 @@
         <v>3</v>
       </c>
       <c r="C22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D22">
         <v>59.859418699999999</v>
@@ -980,7 +980,7 @@
         <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D23">
         <v>59.852781</v>
@@ -1003,7 +1003,7 @@
         <v>3</v>
       </c>
       <c r="C24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D24">
         <v>59.874628700000002</v>
@@ -1026,7 +1026,7 @@
         <v>3</v>
       </c>
       <c r="C25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D25">
         <v>59.871397700000003</v>
@@ -1049,7 +1049,7 @@
         <v>3</v>
       </c>
       <c r="C26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D26">
         <v>59.833032500000002</v>
@@ -1072,7 +1072,7 @@
         <v>3</v>
       </c>
       <c r="C27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D27">
         <v>59.851444700000002</v>
@@ -1095,7 +1095,7 @@
         <v>3</v>
       </c>
       <c r="C28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D28">
         <v>59.856229300000003</v>
@@ -1118,7 +1118,7 @@
         <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D29">
         <v>59.851660199999998</v>
@@ -1141,7 +1141,7 @@
         <v>3</v>
       </c>
       <c r="C30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D30">
         <v>59.893473</v>
@@ -1164,7 +1164,7 @@
         <v>3</v>
       </c>
       <c r="C31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D31">
         <v>59.821291799999997</v>

</xml_diff>

<commit_message>
fix issue with formatting/decimal separator in station.csv/.xlsx
</commit_message>
<xml_diff>
--- a/sql-scripts/station.xlsx
+++ b/sql-scripts/station.xlsx
@@ -143,8 +143,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="[$-409]General"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -212,8 +213,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -237,10 +242,10 @@
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.18"/>
   </cols>
@@ -268,7 +273,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
@@ -278,7 +283,7 @@
       <c r="C2" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>58.393154</v>
       </c>
       <c r="E2" s="0" t="n">

</xml_diff>